<commit_message>
commited dispatcher to repo
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\Contracts Concierge_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC49BCBA-475F-4F5C-B126-E34A05713FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA804325-CF15-4AF6-9559-757D793C39A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15660" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="89">
   <si>
     <t>Name</t>
   </si>
@@ -95,131 +95,202 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction succesful.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Calling Get Transaction Data.</t>
+  </si>
+  <si>
+    <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueFolder</t>
+  </si>
+  <si>
+    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
+  </si>
+  <si>
+    <t>MaxConsecutiveSystemExceptions</t>
+  </si>
+  <si>
+    <t>ExceptionMessage_ConsecutiveErrors</t>
+  </si>
+  <si>
+    <t>RetryNumberGetTransactionItem</t>
+  </si>
+  <si>
+    <t>RetryNumberSetTransactionStatus</t>
+  </si>
+  <si>
+    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
+  </si>
+  <si>
+    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
+  </si>
+  <si>
+    <t>ShouldMarkJobAsFaulted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
+  </si>
+  <si>
+    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
+  </si>
+  <si>
+    <t>Contracts Concierge_Dispatcher</t>
+  </si>
+  <si>
+    <t>Cred_Egnyte</t>
+  </si>
+  <si>
+    <t>G2 Egnyte credentials</t>
+  </si>
+  <si>
+    <t>DefaultDelay</t>
+  </si>
+  <si>
+    <t>ExtraShortTimeout</t>
+  </si>
+  <si>
+    <t>ShortTimeout</t>
+  </si>
+  <si>
+    <t>MediumTimeout</t>
+  </si>
+  <si>
+    <t>LongTimeout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Process delay </t>
+  </si>
+  <si>
+    <t>Process extra short timeout</t>
+  </si>
+  <si>
+    <t>Process short timeout</t>
+  </si>
+  <si>
+    <t>Process medium timeout</t>
+  </si>
+  <si>
+    <t>Process long timeout</t>
+  </si>
+  <si>
+    <t>EgnyteCustomerFolders_URL</t>
+  </si>
+  <si>
+    <t>Egnyte customer folders URL</t>
+  </si>
+  <si>
+    <t>HeaderKeyword_Customers</t>
+  </si>
+  <si>
+    <t>Customers folder header keyword</t>
+  </si>
+  <si>
+    <t>Temporary downloads folder path</t>
+  </si>
+  <si>
+    <t>FilesStorageBucket</t>
+  </si>
+  <si>
+    <t>Storage bucket for downloaded files</t>
+  </si>
+  <si>
+    <t>ExtraLongTimeout</t>
+  </si>
+  <si>
+    <t>Process extra long timeout for downloads</t>
+  </si>
+  <si>
+    <t>IgnoreFileExtensions</t>
+  </si>
+  <si>
+    <t>Ignore file extensions when checking for downloaded folders and files as zip</t>
+  </si>
+  <si>
+    <t>FilterUploadFiles</t>
+  </si>
+  <si>
+    <t>Filter to include these files only in for each file in folder</t>
+  </si>
+  <si>
+    <t>TestingQueue</t>
+  </si>
+  <si>
     <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction succesful.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Calling Get Transaction Data.</t>
-  </si>
-  <si>
-    <t>OrchestratorAssetFolder</t>
-  </si>
-  <si>
-    <t>OrchestratorQueueFolder</t>
-  </si>
-  <si>
-    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
-  </si>
-  <si>
-    <t>MaxConsecutiveSystemExceptions</t>
-  </si>
-  <si>
-    <t>ExceptionMessage_ConsecutiveErrors</t>
-  </si>
-  <si>
-    <t>RetryNumberGetTransactionItem</t>
-  </si>
-  <si>
-    <t>RetryNumberSetTransactionStatus</t>
-  </si>
-  <si>
-    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
-  </si>
-  <si>
-    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
-  </si>
-  <si>
-    <t>ShouldMarkJobAsFaulted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
-  </si>
-  <si>
-    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
-  </si>
-  <si>
-    <t>ProcessABCQueue</t>
-  </si>
-  <si>
-    <t>Contracts Concierge_Dispatcher</t>
-  </si>
-  <si>
-    <t>Cred_Egnyte</t>
-  </si>
-  <si>
-    <t>G2 Egnyte credentials</t>
-  </si>
-  <si>
-    <t>DefaultDelay</t>
-  </si>
-  <si>
-    <t>ExtraShortTimeout</t>
-  </si>
-  <si>
-    <t>ShortTimeout</t>
-  </si>
-  <si>
-    <t>MediumTimeout</t>
-  </si>
-  <si>
-    <t>LongTimeout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Process delay </t>
-  </si>
-  <si>
-    <t>Process extra short timeout</t>
-  </si>
-  <si>
-    <t>Process short timeout</t>
-  </si>
-  <si>
-    <t>Process medium timeout</t>
-  </si>
-  <si>
-    <t>Process long timeout</t>
-  </si>
-  <si>
-    <t>EgnyteCustomerFolders_URL</t>
-  </si>
-  <si>
-    <t>Egnyte customer folders URL</t>
-  </si>
-  <si>
-    <t>HeaderKeyword_Customers</t>
-  </si>
-  <si>
-    <t>Customers folder header keyword</t>
-  </si>
-  <si>
-    <t>DownloadedFilesTempFolderPath</t>
-  </si>
-  <si>
-    <t>Temporary downloads folder path</t>
-  </si>
-  <si>
-    <t>FilesStorageBucket</t>
-  </si>
-  <si>
-    <t>Storage bucket for downloaded files</t>
+  </si>
+  <si>
+    <t>HeaderKeyword_SubmittedContracts</t>
+  </si>
+  <si>
+    <t>Submitted contracts header keyword</t>
+  </si>
+  <si>
+    <t>EgnyteDownloadFolder_URL</t>
+  </si>
+  <si>
+    <t>Egnyte folder URL where to download files from</t>
+  </si>
+  <si>
+    <t>UploadFilesFolder</t>
+  </si>
+  <si>
+    <t>Folder from where the files will be uploaded to the Orchestrator storage bucket</t>
+  </si>
+  <si>
+    <t>TempFolder</t>
+  </si>
+  <si>
+    <t>Temp folder path where files are downloaded and uploaded from</t>
+  </si>
+  <si>
+    <t>DownloadsFolder</t>
+  </si>
+  <si>
+    <t>DispatcherReportName</t>
+  </si>
+  <si>
+    <t>Dispatcher report name</t>
+  </si>
+  <si>
+    <t>UploadedFilesSheet</t>
+  </si>
+  <si>
+    <t>Report uploaded files sheet</t>
+  </si>
+  <si>
+    <t>ZipFilesSheetName</t>
+  </si>
+  <si>
+    <t>Sheet wit zip files list</t>
+  </si>
+  <si>
+    <t>Dispatcher_ReportEmailRecipient</t>
+  </si>
+  <si>
+    <t>Dispatcher report email recipient</t>
+  </si>
+  <si>
+    <t>Dispatcher_ReportEmailSubject</t>
+  </si>
+  <si>
+    <t>Dispatcher report email subject</t>
   </si>
 </sst>
 </file>
@@ -598,7 +669,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -645,10 +716,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -656,11 +727,11 @@
     </row>
     <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -669,7 +740,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -679,13 +750,13 @@
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1743,18 +1814,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1778,7 +1849,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1800,7 +1871,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1811,7 +1882,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1822,53 +1893,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2850,17 +2921,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="31.90625" customWidth="1"/>
-    <col min="2" max="2" width="30.08984375" customWidth="1"/>
-    <col min="3" max="3" width="60.36328125" customWidth="1"/>
+    <col min="2" max="2" width="32.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2872,7 +2943,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -2902,125 +2973,245 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>63</v>
+      <c r="A10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
         <v>64</v>
       </c>
+      <c r="B14" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -3989,6 +4180,9 @@
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
+    <row r="1001" ht="14.25" customHeight="1"/>
+    <row r="1002" ht="14.25" customHeight="1"/>
+    <row r="1003" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added regex assets to config
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\rpa-prc-contracts-concierge-dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A08FE65-00F3-4FFF-942B-C92331D76B2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34823D8D-AB18-4ECC-B1B6-4ED4AC40E18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13140" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="97">
   <si>
     <t>Name</t>
   </si>
@@ -291,6 +291,30 @@
   </si>
   <si>
     <t>Name of downloaded zip of files from Egnyte</t>
+  </si>
+  <si>
+    <t>FileNameRegex</t>
+  </si>
+  <si>
+    <t>Regex used to extract file name from Egnyte</t>
+  </si>
+  <si>
+    <t>EgnyteFilePathRegex</t>
+  </si>
+  <si>
+    <t>Regex used to extract file path from Egnyte</t>
+  </si>
+  <si>
+    <t>LastUpdatedByRegex</t>
+  </si>
+  <si>
+    <t>Regex used to extract the last updated by name from Egnyte</t>
+  </si>
+  <si>
+    <t>ModifiedDateRegex</t>
+  </si>
+  <si>
+    <t>Regex used to extract the modified date from Egnyte</t>
   </si>
 </sst>
 </file>
@@ -2923,8 +2947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -3202,10 +3226,50 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A23" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A24" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A26" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26" t="s">
+        <v>96</v>
+      </c>
+    </row>
     <row r="27" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:4" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
updated config, removed unused code
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\rpa-prc-contracts-concierge-dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34823D8D-AB18-4ECC-B1B6-4ED4AC40E18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55A6267-45AF-4855-AE8E-B495A31F00B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="101">
   <si>
     <t>Name</t>
   </si>
@@ -315,6 +315,18 @@
   </si>
   <si>
     <t>Regex used to extract the modified date from Egnyte</t>
+  </si>
+  <si>
+    <t>RetryScope_RetryNumber</t>
+  </si>
+  <si>
+    <t>Retry scope number of retries</t>
+  </si>
+  <si>
+    <t>RetryScope_RetryInterval</t>
+  </si>
+  <si>
+    <t>Retry scope retry interval</t>
   </si>
 </sst>
 </file>
@@ -2947,8 +2959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -3270,8 +3282,28 @@
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A27" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27" t="s">
+        <v>97</v>
+      </c>
+      <c r="D27" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A28" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" t="s">
+        <v>99</v>
+      </c>
+      <c r="D28" t="s">
+        <v>100</v>
+      </c>
+    </row>
     <row r="29" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="31" spans="1:4" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
mapped arguments to assets, updated config file, enabled disabled code, deleted code that won't be used
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\rpa-prc-contracts-concierge-dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55A6267-45AF-4855-AE8E-B495A31F00B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71B6E94-BDA1-4917-B3AA-14828B65CFF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="97">
   <si>
     <t>Name</t>
   </si>
@@ -191,12 +191,6 @@
     <t>Process long timeout</t>
   </si>
   <si>
-    <t>HeaderKeyword_Customers</t>
-  </si>
-  <si>
-    <t>Customers folder header keyword</t>
-  </si>
-  <si>
     <t>Temporary downloads folder path</t>
   </si>
   <si>
@@ -218,36 +212,12 @@
     <t>Ignore file extensions when checking for downloaded folders and files as zip</t>
   </si>
   <si>
-    <t>FilterUploadFiles</t>
-  </si>
-  <si>
-    <t>Filter to include these files only in for each file in folder</t>
-  </si>
-  <si>
     <t>TestingQueue</t>
   </si>
   <si>
     <t>OrchestratorQueueName</t>
   </si>
   <si>
-    <t>HeaderKeyword_SubmittedContracts</t>
-  </si>
-  <si>
-    <t>Submitted contracts header keyword</t>
-  </si>
-  <si>
-    <t>UploadFilesFolder</t>
-  </si>
-  <si>
-    <t>Folder from where the files will be uploaded to the Orchestrator storage bucket</t>
-  </si>
-  <si>
-    <t>TempFolder</t>
-  </si>
-  <si>
-    <t>Temp folder path where files are downloaded and uploaded from</t>
-  </si>
-  <si>
     <t>DownloadsFolder</t>
   </si>
   <si>
@@ -287,12 +257,6 @@
     <t>URL of Egnyte customers</t>
   </si>
   <si>
-    <t>DownloadedZipFileName</t>
-  </si>
-  <si>
-    <t>Name of downloaded zip of files from Egnyte</t>
-  </si>
-  <si>
     <t>FileNameRegex</t>
   </si>
   <si>
@@ -327,6 +291,30 @@
   </si>
   <si>
     <t>Retry scope retry interval</t>
+  </si>
+  <si>
+    <t>ExtractCustomerPathIndex</t>
+  </si>
+  <si>
+    <t>The Egnyte path index of the customer name that needs to be extracted. The index changes because the path changes between prod and test</t>
+  </si>
+  <si>
+    <t>InScopeFileTypes</t>
+  </si>
+  <si>
+    <t>In scope file types</t>
+  </si>
+  <si>
+    <t>FolderExensions</t>
+  </si>
+  <si>
+    <t>Extensions to check if folder</t>
+  </si>
+  <si>
+    <t>IgnoreFoldersNames</t>
+  </si>
+  <si>
+    <t>Folder names to ignore</t>
   </si>
 </sst>
 </file>
@@ -752,10 +740,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -2957,10 +2945,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -3064,101 +3052,101 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D8" s="2" t="s">
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B9" t="s">
-        <v>68</v>
+      <c r="B9" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>59</v>
+        <v>65</v>
+      </c>
+      <c r="B11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>62</v>
+        <v>72</v>
+      </c>
+      <c r="B12" t="s">
+        <v>72</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D13" t="s">
-        <v>65</v>
+        <v>67</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" s="2" t="s">
-        <v>70</v>
+      <c r="A14" t="s">
+        <v>68</v>
       </c>
       <c r="B14" t="s">
-        <v>70</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
+      </c>
+      <c r="D14" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
@@ -3168,52 +3156,52 @@
       <c r="B16" t="s">
         <v>75</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="2" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
+      </c>
+      <c r="D17" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
+      </c>
+      <c r="D18" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B19" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D19" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B20" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D20" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.25" customHeight="1">
@@ -3223,7 +3211,7 @@
       <c r="B21" t="s">
         <v>85</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" t="s">
         <v>86</v>
       </c>
     </row>
@@ -3234,7 +3222,7 @@
       <c r="B22" t="s">
         <v>87</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" t="s">
         <v>88</v>
       </c>
     </row>
@@ -3282,28 +3270,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A27" t="s">
-        <v>97</v>
-      </c>
-      <c r="B27" t="s">
-        <v>97</v>
-      </c>
-      <c r="D27" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A28" t="s">
-        <v>99</v>
-      </c>
-      <c r="B28" t="s">
-        <v>99</v>
-      </c>
-      <c r="D28" t="s">
-        <v>100</v>
-      </c>
-    </row>
+    <row r="27" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="31" spans="1:4" ht="14.25" customHeight="1"/>
@@ -4271,12 +4239,6 @@
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
-    <row r="1001" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added create downloads folder workflow, removed unused variables and mapped arguments, invoked the workflow in init state
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\rpa-prc-contracts-concierge-dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8B6B31-0750-47A5-B91E-8F945019F8EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84773BC6-5971-4D70-A4BB-1DA435EECB2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2942,7 +2942,7 @@
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
added google drive folder if asset in config, updated workflow test to test sending gmail
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\rpa-prc-contracts-concierge-dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2884690B-5C4E-405C-ABEE-D462F3C9B468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D9FA60-4EF1-4BD2-AB74-E011B08E90CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="98">
   <si>
     <t>Name</t>
   </si>
@@ -312,6 +312,12 @@
   </si>
   <si>
     <t>DU_StorageBucketName</t>
+  </si>
+  <si>
+    <t>GoogleDrive_ReportFolderId</t>
+  </si>
+  <si>
+    <t>Google drive report folder</t>
   </si>
 </sst>
 </file>
@@ -2944,8 +2950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -3256,7 +3262,17 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A26" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
     <row r="27" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:4" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
enabled upload storage file, and enabled delete all files for cleanup at the end
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\rpa-prc-contracts-concierge-dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D9FA60-4EF1-4BD2-AB74-E011B08E90CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED95281-AD63-4E30-B50A-9C175AB2C316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="100">
   <si>
     <t>Name</t>
   </si>
@@ -318,6 +318,12 @@
   </si>
   <si>
     <t>Google drive report folder</t>
+  </si>
+  <si>
+    <t>Dispatcher_ReportEmailBody</t>
+  </si>
+  <si>
+    <t>Dispatcher report email body</t>
   </si>
 </sst>
 </file>
@@ -2950,8 +2956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -3273,7 +3279,17 @@
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A27" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" t="s">
+        <v>98</v>
+      </c>
+      <c r="D27" t="s">
+        <v>99</v>
+      </c>
+    </row>
     <row r="28" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:4" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
updated config file queue name
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\rpa-prc-contracts-concierge-dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED95281-AD63-4E30-B50A-9C175AB2C316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8CE1F0-C594-4A17-A689-C9BE094ED381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -206,9 +206,6 @@
     <t>Process extra long timeout for downloads</t>
   </si>
   <si>
-    <t>TestingQueue</t>
-  </si>
-  <si>
     <t>OrchestratorQueueName</t>
   </si>
   <si>
@@ -324,6 +321,9 @@
   </si>
   <si>
     <t>Dispatcher report email body</t>
+  </si>
+  <si>
+    <t>DU_Queue</t>
   </si>
 </sst>
 </file>
@@ -701,8 +701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -749,10 +749,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>99</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -2956,8 +2956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -3072,10 +3072,10 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>55</v>
@@ -3086,7 +3086,7 @@
         <v>56</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>57</v>
@@ -3094,200 +3094,200 @@
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" t="s">
         <v>63</v>
-      </c>
-      <c r="B10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="B11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="B12" t="s">
-        <v>93</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" t="s">
         <v>65</v>
-      </c>
-      <c r="B13" t="s">
-        <v>65</v>
-      </c>
-      <c r="D13" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" t="s">
         <v>67</v>
-      </c>
-      <c r="B14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="B15" t="s">
-        <v>71</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" t="s">
         <v>73</v>
-      </c>
-      <c r="B16" t="s">
-        <v>73</v>
-      </c>
-      <c r="D16" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1">
       <c r="A17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" t="s">
         <v>75</v>
-      </c>
-      <c r="B17" t="s">
-        <v>75</v>
-      </c>
-      <c r="D17" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25" customHeight="1">
       <c r="A18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" t="s">
         <v>77</v>
-      </c>
-      <c r="B18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D18" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1">
       <c r="A19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" t="s">
         <v>79</v>
-      </c>
-      <c r="B19" t="s">
-        <v>79</v>
-      </c>
-      <c r="D19" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1">
       <c r="A20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" t="s">
         <v>81</v>
-      </c>
-      <c r="B20" t="s">
-        <v>81</v>
-      </c>
-      <c r="D20" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.25" customHeight="1">
       <c r="A21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" t="s">
         <v>83</v>
-      </c>
-      <c r="B21" t="s">
-        <v>83</v>
-      </c>
-      <c r="D21" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14.25" customHeight="1">
       <c r="A22" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" t="s">
         <v>85</v>
-      </c>
-      <c r="B22" t="s">
-        <v>85</v>
-      </c>
-      <c r="D22" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.25" customHeight="1">
       <c r="A23" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23" t="s">
         <v>87</v>
-      </c>
-      <c r="B23" t="s">
-        <v>87</v>
-      </c>
-      <c r="D23" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.25" customHeight="1">
       <c r="A24" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" t="s">
         <v>89</v>
-      </c>
-      <c r="B24" t="s">
-        <v>89</v>
-      </c>
-      <c r="D24" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.25" customHeight="1">
       <c r="A25" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" t="s">
         <v>91</v>
-      </c>
-      <c r="B25" t="s">
-        <v>91</v>
-      </c>
-      <c r="D25" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="14.25" customHeight="1">
       <c r="A26" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="B26" t="s">
-        <v>96</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.25" customHeight="1">
       <c r="A27" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27" t="s">
+        <v>97</v>
+      </c>
+      <c r="D27" t="s">
         <v>98</v>
-      </c>
-      <c r="B27" t="s">
-        <v>98</v>
-      </c>
-      <c r="D27" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
added send email in system exception transaction status
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BogdanJianu\Desktop\Contracts Concierge_Dispatcher\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\rpa-prc-contracts-concierge-dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77EFFCCB-0188-4D73-AD43-D66D7689F669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F16811-99F6-45ED-9AB3-10F7A74191D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="106">
   <si>
     <t>Name</t>
   </si>
@@ -324,6 +324,24 @@
   </si>
   <si>
     <t>Dispatcher report email body</t>
+  </si>
+  <si>
+    <t>EmailRecipient_RpaSupport</t>
+  </si>
+  <si>
+    <t>Rpa team support email recipients</t>
+  </si>
+  <si>
+    <t>DispatcherEmail_Subject_Error</t>
+  </si>
+  <si>
+    <t>Error email subject</t>
+  </si>
+  <si>
+    <t>Dispatcher_ErrorEmail_Body</t>
+  </si>
+  <si>
+    <t>Error email body which contains the exception type, source and message</t>
   </si>
 </sst>
 </file>
@@ -1793,7 +1811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -2956,8 +2974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -3291,9 +3309,39 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A29" t="s">
+        <v>100</v>
+      </c>
+      <c r="B29" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A30" t="s">
+        <v>102</v>
+      </c>
+      <c r="B30" t="s">
+        <v>102</v>
+      </c>
+      <c r="D30" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
+        <v>104</v>
+      </c>
+      <c r="B31" t="s">
+        <v>104</v>
+      </c>
+      <c r="D31" t="s">
+        <v>105</v>
+      </c>
+    </row>
     <row r="32" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="33" customFormat="1" ht="14.25" customHeight="1"/>
     <row r="34" customFormat="1" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
added send email when no report is created
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\rpa-prc-contracts-concierge-dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F16811-99F6-45ED-9AB3-10F7A74191D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96129BD7-2F6B-48A4-88F4-AAC7040E5342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="108">
   <si>
     <t>Name</t>
   </si>
@@ -342,6 +342,12 @@
   </si>
   <si>
     <t>Error email body which contains the exception type, source and message</t>
+  </si>
+  <si>
+    <t>Dispatcher_EmailBody_NoReport</t>
+  </si>
+  <si>
+    <t>Email body when no report has been created</t>
   </si>
 </sst>
 </file>
@@ -2974,8 +2980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -3342,7 +3348,17 @@
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B32" t="s">
+        <v>106</v>
+      </c>
+      <c r="D32" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="33" customFormat="1" ht="14.25" customHeight="1"/>
     <row r="34" customFormat="1" ht="14.25" customHeight="1"/>
     <row r="35" customFormat="1" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
updated send email components
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willa\source\repos\rpa-prc-contracts-concierge-dispatcher\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\rpa-prc-contracts-concierge-dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E98472-D925-4849-8C43-448AD6E56D08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B87E14F-3B80-41EC-871B-95FAD1CAA56B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="111">
   <si>
     <t>Name</t>
   </si>
@@ -351,6 +351,12 @@
   </si>
   <si>
     <t>Contracts Concierge/Prod</t>
+  </si>
+  <si>
+    <t>CustomerName_SplitKeyword</t>
+  </si>
+  <si>
+    <t>Keyword used to split the Egnyte file path to extract the customer name</t>
   </si>
 </sst>
 </file>
@@ -728,16 +734,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -785,7 +791,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
@@ -797,7 +803,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1826,12 +1832,12 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1868,7 +1874,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1879,7 +1885,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1993,7 +1999,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -2983,18 +2989,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="32.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.90625" customWidth="1"/>
+    <col min="2" max="2" width="32.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3397,61 +3403,74 @@
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A28" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" t="s">
+        <v>108</v>
+      </c>
+      <c r="D28" t="s">
+        <v>101</v>
+      </c>
+    </row>
     <row r="29" spans="1:4" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B29" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C29" t="s">
         <v>108</v>
       </c>
       <c r="D29" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B30" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C30" t="s">
         <v>108</v>
       </c>
       <c r="D30" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B31" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C31" t="s">
         <v>108</v>
       </c>
       <c r="D31" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B32" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C32" t="s">
         <v>108</v>
       </c>
       <c r="D32" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" ht="14.25" customHeight="1"/>
@@ -4421,7 +4440,6 @@
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated config file by removing folder address and making the du queue and orch folder assets
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\rpa-prc-contracts-concierge-dispatcher\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BogdanJianu\Desktop\rpa-prc-contracts-concierge-dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B87E14F-3B80-41EC-871B-95FAD1CAA56B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F53339E-C77F-4C18-B325-99D9059086AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="109">
   <si>
     <t>Name</t>
   </si>
@@ -85,10 +85,6 @@
   </si>
   <si>
     <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
@@ -155,9 +151,6 @@
     <t>OrchestratorQueueName</t>
   </si>
   <si>
-    <t>DU_Queue</t>
-  </si>
-  <si>
     <t>Contracts Concierge_Dispatcher</t>
   </si>
   <si>
@@ -350,13 +343,13 @@
     <t>Email body when no report has been created</t>
   </si>
   <si>
-    <t>Contracts Concierge/Prod</t>
-  </si>
-  <si>
     <t>CustomerName_SplitKeyword</t>
   </si>
   <si>
     <t>Keyword used to split the Egnyte file path to extract the customer name</t>
+  </si>
+  <si>
+    <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
   </si>
 </sst>
 </file>
@@ -724,7 +717,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -732,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z993"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -780,53 +773,33 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:26" ht="29">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="43.5">
-      <c r="A3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>30</v>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="29">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1812,11 +1785,6 @@
     <row r="991" ht="14.25" customHeight="1"/>
     <row r="992" ht="14.25" customHeight="1"/>
     <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1882,18 +1850,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1917,7 +1885,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1939,7 +1907,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1950,7 +1918,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1961,53 +1929,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2991,8 +2959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -3011,7 +2979,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -3041,454 +3009,383 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" t="s">
-        <v>108</v>
+        <v>45</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" t="s">
-        <v>108</v>
+        <v>47</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" t="s">
-        <v>108</v>
+        <v>49</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" t="s">
-        <v>108</v>
+        <v>51</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" t="s">
-        <v>108</v>
+        <v>53</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" t="s">
-        <v>108</v>
+        <v>55</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" t="s">
-        <v>108</v>
+        <v>57</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" t="s">
-        <v>108</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" t="s">
-        <v>108</v>
+        <v>62</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" t="s">
-        <v>108</v>
+        <v>64</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
-      </c>
-      <c r="C12" t="s">
-        <v>108</v>
+        <v>66</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C13" t="s">
-        <v>108</v>
+        <v>68</v>
       </c>
       <c r="D13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" t="s">
-        <v>108</v>
+        <v>70</v>
       </c>
       <c r="D14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
-      </c>
-      <c r="C15" t="s">
-        <v>108</v>
+        <v>72</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
-      </c>
-      <c r="C16" t="s">
-        <v>108</v>
+        <v>74</v>
       </c>
       <c r="D16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B17" t="s">
-        <v>78</v>
-      </c>
-      <c r="C17" t="s">
-        <v>108</v>
+        <v>76</v>
       </c>
       <c r="D17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B18" t="s">
-        <v>80</v>
-      </c>
-      <c r="C18" t="s">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="D18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B19" t="s">
-        <v>82</v>
-      </c>
-      <c r="C19" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="D19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B20" t="s">
-        <v>84</v>
-      </c>
-      <c r="C20" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="D20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B21" t="s">
-        <v>86</v>
-      </c>
-      <c r="C21" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="D21" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B22" t="s">
-        <v>88</v>
-      </c>
-      <c r="C22" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="D22" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B23" t="s">
-        <v>90</v>
-      </c>
-      <c r="C23" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="D23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B24" t="s">
-        <v>92</v>
-      </c>
-      <c r="C24" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="D24" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B25" t="s">
-        <v>94</v>
-      </c>
-      <c r="C25" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="D25" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="14.25" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B26" t="s">
-        <v>96</v>
-      </c>
-      <c r="C26" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B27" t="s">
-        <v>98</v>
-      </c>
-      <c r="C27" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="D27" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B28" t="s">
-        <v>100</v>
-      </c>
-      <c r="C28" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="D28" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B29" t="s">
-        <v>102</v>
-      </c>
-      <c r="C29" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D29" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B30" t="s">
-        <v>104</v>
-      </c>
-      <c r="C30" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D30" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B31" t="s">
-        <v>106</v>
-      </c>
-      <c r="C31" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D31" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B32" t="s">
-        <v>109</v>
-      </c>
-      <c r="C32" t="s">
+        <v>106</v>
+      </c>
+      <c r="D32" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A33" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="2"/>
+      <c r="D33" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A34" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D32" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+    </row>
+    <row r="35" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="36" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="37" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="38" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="39" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
added ignoretempfileextenstions asset in config
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BogdanJianu\Desktop\rpa-prc-contracts-concierge-dispatcher\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\rpa-prc-contracts-concierge-dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F53339E-C77F-4C18-B325-99D9059086AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9B85B3-715D-42C8-95B4-A93E4CCC0AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7530" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="111">
   <si>
     <t>Name</t>
   </si>
@@ -350,6 +350,12 @@
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
+  </si>
+  <si>
+    <t>IgnoreTempFileExtensions</t>
+  </si>
+  <si>
+    <t>Temp file extensions to be ignored by the wait for download activity</t>
   </si>
 </sst>
 </file>
@@ -727,7 +733,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z993"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -2959,8 +2965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -3372,7 +3378,17 @@
         <v>108</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="35" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A35" t="s">
+        <v>109</v>
+      </c>
+      <c r="B35" t="s">
+        <v>109</v>
+      </c>
+      <c r="D35" t="s">
+        <v>110</v>
+      </c>
+    </row>
     <row r="36" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="37" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="38" spans="1:4" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
changed du queue asset name in config to DocumentUnderstandingQueueName
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\rpa-prc-contracts-concierge-dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9B85B3-715D-42C8-95B4-A93E4CCC0AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A12AFA-B68E-4953-BAEA-61DCFE439E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7530" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-45" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="112">
   <si>
     <t>Name</t>
   </si>
@@ -356,6 +356,9 @@
   </si>
   <si>
     <t>Temp file extensions to be ignored by the wait for download activity</t>
+  </si>
+  <si>
+    <t>DocumentUnderstandingQueueName</t>
   </si>
 </sst>
 </file>
@@ -2965,8 +2968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -3371,7 +3374,7 @@
         <v>41</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>41</v>
+        <v>111</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">

</xml_diff>